<commit_message>
:Heavy_plus_sign: Added shallow lakes
</commit_message>
<xml_diff>
--- a/Lab meeting presentation/Tableau confusion et resume.xlsx
+++ b/Lab meeting presentation/Tableau confusion et resume.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Postdoc\UdeM\Github\US_LakeProfiles\Lab meeting presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E479E9-DCF8-4CF5-BE25-09D7B454E199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10BE19BB-DECE-434B-B26E-4B5FC08CD700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{FD1CFFE2-5CE0-4276-953F-BDA3A8A35B6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FD1CFFE2-5CE0-4276-953F-BDA3A8A35B6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t>Predicted</t>
   </si>
@@ -119,18 +120,9 @@
     <t>Murky</t>
   </si>
   <si>
-    <t>217 (59%)</t>
-  </si>
-  <si>
     <t>26 (7%)</t>
   </si>
   <si>
-    <t>21 (6%)</t>
-  </si>
-  <si>
-    <t>105 (28%)</t>
-  </si>
-  <si>
     <t>RF bin hypo</t>
   </si>
   <si>
@@ -149,18 +141,6 @@
     <t>RF bin hypox</t>
   </si>
   <si>
-    <t>17 (9%)</t>
-  </si>
-  <si>
-    <t>43 (23%)</t>
-  </si>
-  <si>
-    <t>20 (11%)</t>
-  </si>
-  <si>
-    <t>110 (58%)</t>
-  </si>
-  <si>
     <t>45 (23%)</t>
   </si>
   <si>
@@ -171,6 +151,63 @@
   </si>
   <si>
     <t>105 (58%)</t>
+  </si>
+  <si>
+    <t>Reg log bin hypo (lasso min)</t>
+  </si>
+  <si>
+    <t>231 (62%)</t>
+  </si>
+  <si>
+    <t>48 (13%)</t>
+  </si>
+  <si>
+    <t>7 (2%)</t>
+  </si>
+  <si>
+    <t>83 (22%)</t>
+  </si>
+  <si>
+    <t>Reg log bin hypox (lasso min)</t>
+  </si>
+  <si>
+    <t>13 (9%)</t>
+  </si>
+  <si>
+    <t>30 (21%)</t>
+  </si>
+  <si>
+    <t>28 (20%)</t>
+  </si>
+  <si>
+    <t>72 (5%)</t>
+  </si>
+  <si>
+    <t>43 (9.1%)</t>
+  </si>
+  <si>
+    <t>126 (26.6%)</t>
+  </si>
+  <si>
+    <t>42 (8.8%)</t>
+  </si>
+  <si>
+    <t>264 (55.5%)</t>
+  </si>
+  <si>
+    <t>Nr (%)</t>
+  </si>
+  <si>
+    <t>109 (8.9%)</t>
+  </si>
+  <si>
+    <t>70 (5.7%)</t>
+  </si>
+  <si>
+    <t>367 (29.8%)</t>
+  </si>
+  <si>
+    <t>684 (55.6%)</t>
   </si>
 </sst>
 </file>
@@ -276,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -303,10 +340,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -325,9 +377,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -336,6 +385,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF000000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -348,7 +402,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -644,13 +698,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA07803B-1F0F-43A6-A946-0ED1F58636F4}">
-  <dimension ref="A2:AA13"/>
+  <dimension ref="A2:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="A3" sqref="A3:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" customWidth="1"/>
@@ -666,25 +720,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="H2" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="22"/>
+      <c r="B2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="H2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="20"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
       <c r="V2" s="6" t="s">
         <v>15</v>
       </c>
@@ -700,33 +754,33 @@
     <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="18"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="15"/>
+      <c r="J3" s="18"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16" t="s">
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16" t="s">
+      <c r="S3" s="21"/>
+      <c r="T3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="16"/>
+      <c r="U3" s="21"/>
       <c r="V3" s="7"/>
-      <c r="X3" s="14" t="s">
+      <c r="X3" s="19" t="s">
         <v>19</v>
       </c>
       <c r="Y3" s="12" t="s">
@@ -756,27 +810,27 @@
       <c r="J4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="20" t="s">
+      <c r="O4" s="24"/>
+      <c r="P4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="20" t="s">
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="U4" s="21"/>
+      <c r="U4" s="26"/>
       <c r="V4" s="8">
         <v>0.85</v>
       </c>
-      <c r="X4" s="14"/>
+      <c r="X4" s="19"/>
       <c r="Y4" s="12" t="s">
         <v>25</v>
       </c>
@@ -788,49 +842,49 @@
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="19" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="22"/>
+      <c r="N5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="20" t="s">
+      <c r="O5" s="24"/>
+      <c r="P5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="20" t="s">
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="U5" s="21"/>
+      <c r="U5" s="26"/>
       <c r="V5" s="8">
         <v>0.59</v>
       </c>
-      <c r="X5" s="14"/>
+      <c r="X5" s="19"/>
       <c r="Y5" s="12" t="s">
         <v>26</v>
       </c>
@@ -842,49 +896,49 @@
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="14"/>
+        <v>56</v>
+      </c>
+      <c r="G6" s="19"/>
       <c r="H6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="19"/>
-      <c r="P6" s="20" t="s">
+      <c r="O6" s="24"/>
+      <c r="P6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="20" t="s">
+      <c r="Q6" s="26"/>
+      <c r="R6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="S6" s="21"/>
-      <c r="T6" s="20" t="s">
+      <c r="S6" s="26"/>
+      <c r="T6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="U6" s="21"/>
+      <c r="U6" s="26"/>
       <c r="V6" s="8">
         <v>0.81</v>
       </c>
-      <c r="X6" s="14"/>
+      <c r="X6" s="19"/>
       <c r="Y6" s="12" t="s">
         <v>27</v>
       </c>
@@ -896,46 +950,46 @@
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="M7" s="17"/>
-      <c r="N7" s="18" t="s">
+      <c r="M7" s="22"/>
+      <c r="N7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="20" t="s">
+      <c r="O7" s="24"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="U7" s="21"/>
+      <c r="U7" s="26"/>
       <c r="V7" s="8">
         <v>0.47</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B9" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="H9" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="22"/>
+      <c r="B9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="H9" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="15"/>
+      <c r="D10" s="18"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="15"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
@@ -958,76 +1012,198 @@
       <c r="U11" s="5"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>2</v>
       </c>
       <c r="I12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="G15" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+    </row>
+    <row r="16" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="19"/>
+      <c r="B19" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="D19" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="9" t="s">
+      <c r="G19" s="19"/>
+      <c r="H19" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="15" t="s">
         <v>45</v>
       </c>
+      <c r="J19" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="18"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G23" s="1"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G24" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G25" s="19"/>
+      <c r="H25" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R4:S4"/>
+  <mergeCells count="43">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G15:J15"/>
     <mergeCell ref="X3:X6"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A5:A6"/>
@@ -1042,6 +1218,30 @@
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="T7:U7"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>